<commit_message>
Actualizaciones Analisis de datos Google
</commit_message>
<xml_diff>
--- a/Google/Certificado profesional de Análisis de datos de Google/1. Foundations. Data, Data, Everywhere/Recolección de datos, TP.xlsx
+++ b/Google/Certificado profesional de Análisis de datos de Google/1. Foundations. Data, Data, Everywhere/Recolección de datos, TP.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15180" yWindow="460" windowWidth="13620" windowHeight="16540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Date</t>
   </si>
@@ -43,17 +43,34 @@
   <si>
     <t>AHT/mins</t>
   </si>
+  <si>
+    <t>total</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -77,11 +94,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -94,6 +113,926 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-CO"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES_tradnl"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Calls</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja1!$A$2:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>44490.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44491.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44492.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44493.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44494.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44495.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44496.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44497.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44498.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44499.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44500.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44501.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44502.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44503.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44504.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$B$2:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>25.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="-2062779312"/>
+        <c:axId val="-2093515456"/>
+      </c:barChart>
+      <c:dateAx>
+        <c:axId val="-2062779312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES_tradnl"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2093515456"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="-2093515456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES_tradnl"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2062779312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES_tradnl"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -359,10 +1298,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -469,7 +1408,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="3">
-        <f t="shared" ref="E5:E14" si="2">D5*B5</f>
+        <f t="shared" ref="E5:E12" si="2">D5*B5</f>
         <v>0</v>
       </c>
       <c r="F5" s="2">
@@ -653,10 +1592,10 @@
       <c r="A14" s="1">
         <v>44502</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="4">
         <v>24</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="4">
         <v>336.61</v>
       </c>
       <c r="D14" s="2">
@@ -676,34 +1615,46 @@
       <c r="A15" s="1">
         <v>44503</v>
       </c>
+      <c r="B15" s="4">
+        <v>24</v>
+      </c>
+      <c r="C15" s="4">
+        <v>336.61</v>
+      </c>
       <c r="D15" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5.6101666666666672</v>
       </c>
       <c r="E15" s="3">
         <f t="shared" ref="E15:E23" si="3">D15*B15</f>
-        <v>0</v>
+        <v>134.64400000000001</v>
       </c>
       <c r="F15" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.2440666666666669</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>44504</v>
       </c>
+      <c r="B16">
+        <v>25</v>
+      </c>
+      <c r="C16">
+        <v>384.76</v>
+      </c>
       <c r="D16" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.4126666666666665</v>
       </c>
       <c r="E16" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>160.31666666666666</v>
       </c>
       <c r="F16" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.6719444444444442</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -825,7 +1776,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="24" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24">
+        <f>SUM(B2:B16)</f>
+        <v>311</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>